<commit_message>
Import input xlsx format correctly for 1 sheet  	modified:   demo.docx  	modified:   input.xlsx  	modified:   testDocx.py
</commit_message>
<xml_diff>
--- a/horoGen/input.xlsx
+++ b/horoGen/input.xlsx
@@ -15,9 +15,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="3">
   <si>
     <t>Section</t>
+  </si>
+  <si>
+    <t>Đường đi</t>
   </si>
   <si>
     <t>Section Name</t>
@@ -33,6 +36,7 @@
   <fonts count="4">
     <font>
       <name val="Arial"/>
+      <charset val="1"/>
       <family val="2"/>
       <sz val="10"/>
     </font>
@@ -113,17 +117,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="B4" activeCellId="0" pane="topLeft" sqref="B4"/>
+      <selection activeCell="B1" activeCellId="0" pane="topLeft" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5764705882353"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.6941176470588"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="1">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="1">
       <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
@@ -131,7 +135,7 @@
         <v>1</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="2">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="2">
       <c r="A2" s="0" t="n">
         <v>1.1</v>
       </c>
@@ -139,7 +143,7 @@
         <v>1</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="3">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="3">
       <c r="A3" s="0" t="n">
         <v>1.2</v>
       </c>
@@ -147,9 +151,44 @@
         <v>1</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="4">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="4">
       <c r="A4" s="0" t="n">
         <v>1.3</v>
+      </c>
+      <c r="B4" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="5">
+      <c r="A5" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="6">
+      <c r="A6" s="0" t="n">
+        <v>1.1</v>
+      </c>
+      <c r="B6" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="7">
+      <c r="A7" s="0" t="n">
+        <v>1.2</v>
+      </c>
+      <c r="B7" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="8">
+      <c r="A8" s="0" t="n">
+        <v>1.3</v>
+      </c>
+      <c r="B8" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
First dev release, accepted output   On branch master  	modified:   demo.docx  	new file:   horoscope.py  	new file:   inotify.sh  	modified:   input.xlsx  	new file:   sample.docx  	new file:   sample.xlsx  	deleted:    testDocx.py  	new file:   test_horoscope.py
</commit_message>
<xml_diff>
--- a/horoGen/input.xlsx
+++ b/horoGen/input.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="198" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="395" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,10 +20,10 @@
     <t>Section</t>
   </si>
   <si>
-    <t>Đường đi</t>
+    <t>Tình yêu</t>
   </si>
   <si>
-    <t>Section Name</t>
+    <t>Tình bạn</t>
   </si>
 </sst>
 </file>
@@ -120,11 +120,11 @@
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="B1" activeCellId="0" pane="topLeft" sqref="B1"/>
+      <selection activeCell="B5" activeCellId="0" pane="topLeft" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.6941176470588"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.8117647058824"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="1">
@@ -148,15 +148,15 @@
         <v>1.2</v>
       </c>
       <c r="B3" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="4">
       <c r="A4" s="0" t="n">
-        <v>1.3</v>
+        <v>2.1</v>
       </c>
       <c r="B4" s="0" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="5">
@@ -169,7 +169,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="6">
       <c r="A6" s="0" t="n">
-        <v>1.1</v>
+        <v>3.1</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>1</v>
@@ -177,18 +177,18 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="7">
       <c r="A7" s="0" t="n">
-        <v>1.2</v>
+        <v>3.2</v>
       </c>
       <c r="B7" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="8">
       <c r="A8" s="0" t="n">
-        <v>1.3</v>
+        <v>4.1</v>
       </c>
       <c r="B8" s="0" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add main application & sample input   On branch master  	modified:   input.xlsx  	new file:   main.py
</commit_message>
<xml_diff>
--- a/horoGen/input.xlsx
+++ b/horoGen/input.xlsx
@@ -5,17 +5,18 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="395" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="1" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="395" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Chau Hoang" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Châu Hoàng" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="3">
   <si>
     <t>Section</t>
   </si>
@@ -119,12 +120,12 @@
   </sheetPr>
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="B5" activeCellId="0" pane="topLeft" sqref="B5"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.8117647058824"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.9294117647059"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="1">
@@ -200,4 +201,102 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B9"/>
+  <sheetViews>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="B9" activeCellId="0" pane="topLeft" sqref="B9"/>
+    </sheetView>
+  </sheetViews>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.6313725490196"/>
+  </cols>
+  <sheetData>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="1">
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="2">
+      <c r="A2" s="0" t="n">
+        <v>1.1</v>
+      </c>
+      <c r="B2" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="3">
+      <c r="A3" s="0" t="n">
+        <v>1.2</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="4">
+      <c r="A4" s="0" t="n">
+        <v>2.1</v>
+      </c>
+      <c r="B4" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="5">
+      <c r="A5" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="6">
+      <c r="A6" s="0" t="n">
+        <v>3.1</v>
+      </c>
+      <c r="B6" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="7">
+      <c r="A7" s="0" t="n">
+        <v>3.2</v>
+      </c>
+      <c r="B7" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="8">
+      <c r="A8" s="0" t="n">
+        <v>4.1</v>
+      </c>
+      <c r="B8" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="9">
+      <c r="A9" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B9" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>